<commit_message>
adjusted eval parameters, added loader for external evaluation
</commit_message>
<xml_diff>
--- a/output_MTW.xlsx
+++ b/output_MTW.xlsx
@@ -348,63 +348,63 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="B1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1">
+        <v>42</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+      <c r="J1">
+        <v>0</v>
+      </c>
+      <c r="K1">
+        <v>0</v>
+      </c>
+      <c r="L1">
+        <v>0</v>
+      </c>
+      <c r="M1">
+        <v>0</v>
+      </c>
+      <c r="N1">
+        <v>0</v>
+      </c>
+      <c r="O1">
+        <v>0</v>
+      </c>
+      <c r="P1">
         <v>13</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1">
-        <v>0</v>
-      </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1">
-        <v>0</v>
-      </c>
-      <c r="J1">
-        <v>0</v>
-      </c>
-      <c r="K1">
-        <v>0</v>
-      </c>
-      <c r="L1">
-        <v>0</v>
-      </c>
-      <c r="M1">
-        <v>0</v>
-      </c>
-      <c r="N1">
-        <v>0</v>
-      </c>
-      <c r="O1">
-        <v>0</v>
-      </c>
-      <c r="P1">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B2">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -443,18 +443,18 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>8</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -507,13 +507,13 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -543,7 +543,7 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -560,10 +560,10 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -593,7 +593,7 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -613,7 +613,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -643,7 +643,7 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>23</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -666,13 +666,13 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -693,7 +693,7 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -716,13 +716,13 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -743,7 +743,7 @@
         <v>0</v>
       </c>
       <c r="P8">
-        <v>40</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -766,13 +766,13 @@
         <v>0</v>
       </c>
       <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
         <v>1</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
       <c r="I9">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -793,7 +793,7 @@
         <v>0</v>
       </c>
       <c r="P9">
-        <v>19</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -825,13 +825,13 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -843,7 +843,7 @@
         <v>0</v>
       </c>
       <c r="P10">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -875,13 +875,13 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -893,7 +893,7 @@
         <v>0</v>
       </c>
       <c r="P11">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -925,13 +925,13 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -943,7 +943,7 @@
         <v>0</v>
       </c>
       <c r="P12">
-        <v>14</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -984,16 +984,16 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="N13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O13">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="P13">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1037,13 +1037,13 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P14">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1087,60 +1087,60 @@
         <v>0</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="P15">
-        <v>22</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="B16">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C16">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="G16">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I16">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="K16">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="L16">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="M16">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="N16">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="O16">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="P16">
         <v>0</v>

</xml_diff>